<commit_message>
Class dataPrep working as expected. Fix syntax errors and other bugs.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Directory where the input image sequence is located.</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>/home/utkarsh/Desktop/testUpload</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Dropbox/Utkarsh/testUpload</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Downloads/cifar-10-python.tar.gz</t>
+  </si>
+  <si>
+    <t>/home/utkarsh/Dropbox/Utkarsh</t>
   </si>
 </sst>
 </file>
@@ -155,10 +164,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -202,6 +211,88 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -211,97 +302,24 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,24 +333,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,6 +368,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -371,13 +392,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,157 +548,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,6 +577,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -580,32 +604,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -625,32 +640,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,147 +659,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1938,7 +1947,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1959,12 +1968,22 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" ht="25.5"/>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fix tqdm import error in uploadFiles() in dropboxAPI class.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Directory which you want to archive</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>File with path which you want to join</t>
+  </si>
+  <si>
+    <t>Delete flag (Set to 1 if you want to delete the split files after combining. 0 otherwise. Default is 1)</t>
   </si>
   <si>
     <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted.zip_split_0001</t>
@@ -51,6 +54,12 @@
   <si>
     <t>/home/utkarsh/Dropbox/Utkarsh</t>
   </si>
+  <si>
+    <t>/home/utkarsh/Desktop/testUpload/01_HM_badChip_wet_bulk_converted.zip_split_0001</t>
+  </si>
+  <si>
+    <t>/Utkarsh/testUpload</t>
+  </si>
 </sst>
 </file>
 
@@ -59,8 +68,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -90,6 +99,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -98,7 +153,68 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,117 +228,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -235,19 +244,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,163 +394,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,13 +453,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -479,11 +492,46 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,186 +550,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1244,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1252,7 +1261,7 @@
     </row>
     <row r="2" ht="25.5" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1428,10 +1437,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1439,18 +1448,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1462,15 +1471,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="50.375" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
@@ -1479,29 +1488,21 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" ht="25.5" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete the original file after upload to Dropbox is complete using API.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Directory which you want to archive</t>
   </si>
@@ -55,10 +55,10 @@
     <t>/home/utkarsh/Dropbox/Utkarsh</t>
   </si>
   <si>
-    <t>/home/utkarsh/Desktop/testUpload/01_HM_badChip_wet_bulk_converted.zip_split_0001</t>
+    <t>/Utkarsh/testUpload</t>
   </si>
   <si>
-    <t>/Utkarsh/testUpload</t>
+    <t>/Utkarsh</t>
   </si>
 </sst>
 </file>
@@ -66,10 +66,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -91,74 +91,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -167,9 +99,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,6 +121,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -191,30 +183,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,8 +212,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,187 +244,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,17 +453,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,22 +501,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,108 +539,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -660,43 +660,43 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1471,15 +1471,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="50.375" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.375" style="2" customWidth="1"/>
@@ -1497,11 +1497,19 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" ht="25.5" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete the sheet for zip folders. It has moved to preProcess folder.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,29 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12345" tabRatio="779" activeTab="2"/>
+    <workbookView windowWidth="24000" windowHeight="9795" tabRatio="779"/>
   </bookViews>
   <sheets>
-    <sheet name="archiveFolder" sheetId="11" r:id="rId1"/>
-    <sheet name="joinFiles" sheetId="13" r:id="rId2"/>
-    <sheet name="dropboxUpload_APP" sheetId="14" r:id="rId3"/>
-    <sheet name="dropboxUpload_API" sheetId="15" r:id="rId4"/>
+    <sheet name="joinFiles" sheetId="13" r:id="rId1"/>
+    <sheet name="dropboxUpload_APP" sheetId="14" r:id="rId2"/>
+    <sheet name="dropboxUpload_API" sheetId="15" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
-  <si>
-    <t>Directory which you want to archive</t>
-  </si>
-  <si>
-    <t>Delete flag (Set to 1 if you want to delete the directory after archiving. 0 otherwise. Default is 0)</t>
-  </si>
-  <si>
-    <t>/home/utkarsh/Desktop/restorePillars/LC2/01_HM_badChip_wet_bulk_converted/npy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>File with path which you want to join</t>
   </si>
@@ -63,10 +53,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -88,8 +78,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -102,41 +100,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -148,6 +116,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -179,29 +170,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -209,24 +215,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,79 +231,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,103 +405,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,6 +440,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -461,15 +460,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,6 +489,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -513,17 +518,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,31 +537,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -570,130 +560,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1043,10 +1033,10 @@
   <sheetPr/>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1229,197 +1219,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
-  <cols>
-    <col min="1" max="1" width="50.3333333333333" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.2190476190476" style="6" customWidth="1"/>
-    <col min="3" max="4" width="15.3333333333333" style="2" customWidth="1"/>
-    <col min="5" max="16378" width="9" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="89.25" spans="1:5">
-      <c r="A1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="25.5" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1434,10 +1236,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1445,10 +1247,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1457,7 +1259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E3"/>
@@ -1477,10 +1279,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1488,18 +1290,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entries for new batch of upload.
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="11655" tabRatio="779" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7790" tabRatio="779" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="joinFiles" sheetId="13" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>File with path which you want to join</t>
   </si>
@@ -33,13 +33,10 @@
     <t>Folder where you want to upload it on Dropbox</t>
   </si>
   <si>
-    <t>E:\seewee</t>
+    <t>Z:\xiangwen</t>
   </si>
   <si>
-    <t>E:\Dropbox (NUSCentreofBioImagin)\Backup\seewee\krakenBackup</t>
-  </si>
-  <si>
-    <t>Z:\utkarsh\seewee</t>
+    <t>E:\Dropbox (NUSCentreofBioImagin)\Backup\xiangwen</t>
   </si>
   <si>
     <t>/mnt/d/Projects/Datasets/Vehicles/non-vehicles</t>
@@ -56,10 +53,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -81,6 +78,50 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -89,30 +130,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,18 +191,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -162,68 +221,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -234,13 +231,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,169 +399,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,69 +436,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,153 +474,216 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1042,15 +1039,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="50.3333333333333" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.2190476190476" style="6" customWidth="1"/>
-    <col min="3" max="4" width="15.3333333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="50.3363636363636" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.2181818181818" style="6" customWidth="1"/>
+    <col min="3" max="4" width="15.3363636363636" style="2" customWidth="1"/>
     <col min="5" max="16378" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="89.25" spans="1:5">
+    <row r="1" ht="78" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1058,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" ht="25.5" spans="1:4">
+    <row r="2" ht="25" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1222,18 +1219,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="50.3333333333333" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.3333333333333" style="2" customWidth="1"/>
+    <col min="1" max="2" width="50.3363636363636" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.3363636363636" style="2" customWidth="1"/>
     <col min="5" max="16378" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -1248,19 +1245,11 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" ht="25.5" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" ht="25.5" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1281,10 +1270,10 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="50.3333333333333" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.3333333333333" style="2" customWidth="1"/>
+    <col min="1" max="2" width="50.3363636363636" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.3363636363636" style="2" customWidth="1"/>
     <col min="5" max="16378" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -1301,18 +1290,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>